<commit_message>
added Hikurangi from Clark et al. (2021)
</commit_message>
<xml_diff>
--- a/data_compilation.xlsx
+++ b/data_compilation.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adminalba/Documents/Paleoseismology compilation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333630A2-E069-544C-8EB4-784D4D3FC3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4582212C-32D9-4845-8D27-2109524BBDDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{0C72CEA8-103F-664E-BFC3-8082C479B46F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="149">
   <si>
     <t>Year</t>
   </si>
@@ -453,6 +453,36 @@
   </si>
   <si>
     <t>Type_lat_lon</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>Clark et al. 2019</t>
+  </si>
+  <si>
+    <t>Hikurangi</t>
+  </si>
+  <si>
+    <t>Central</t>
+  </si>
+  <si>
+    <t>Central, northern</t>
+  </si>
+  <si>
+    <t>Southern, central, northern</t>
+  </si>
+  <si>
+    <t>Southern transitional, southern, central</t>
+  </si>
+  <si>
+    <t>Southern, central</t>
+  </si>
+  <si>
+    <t>Southern transitional, southern, central, northern</t>
+  </si>
+  <si>
+    <t>Southern transitional, southern</t>
   </si>
 </sst>
 </file>
@@ -824,10 +854,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B2C05D8-0418-284A-9032-08A034BF23B3}">
-  <dimension ref="A1:I199"/>
+  <dimension ref="A1:I209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="G216" sqref="G216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6126,6 +6156,280 @@
         <v>123</v>
       </c>
     </row>
+    <row r="200" spans="1:9">
+      <c r="A200">
+        <f>1950-7000</f>
+        <v>-5050</v>
+      </c>
+      <c r="B200">
+        <f>(-39.81635166+-39.66777892)/2</f>
+        <v>-39.742065289999999</v>
+      </c>
+      <c r="C200">
+        <v>-39.104548110000003</v>
+      </c>
+      <c r="D200" t="s">
+        <v>139</v>
+      </c>
+      <c r="F200" t="s">
+        <v>140</v>
+      </c>
+      <c r="G200" t="s">
+        <v>141</v>
+      </c>
+      <c r="H200" t="s">
+        <v>142</v>
+      </c>
+      <c r="I200" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9">
+      <c r="A201">
+        <f>1950-5500</f>
+        <v>-3550</v>
+      </c>
+      <c r="B201">
+        <f>(-39.81635166+-39.66777892)/2</f>
+        <v>-39.742065289999999</v>
+      </c>
+      <c r="C201">
+        <v>-38.531135749999997</v>
+      </c>
+      <c r="D201" t="s">
+        <v>139</v>
+      </c>
+      <c r="F201" t="s">
+        <v>140</v>
+      </c>
+      <c r="G201" t="s">
+        <v>141</v>
+      </c>
+      <c r="H201" t="s">
+        <v>143</v>
+      </c>
+      <c r="I201" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9">
+      <c r="A202">
+        <f>1950-4800</f>
+        <v>-2850</v>
+      </c>
+      <c r="B202">
+        <v>-39.816351660000002</v>
+      </c>
+      <c r="C202">
+        <f>(-38.68182995+-38.55154665)/2</f>
+        <v>-38.6166883</v>
+      </c>
+      <c r="D202" t="s">
+        <v>139</v>
+      </c>
+      <c r="F202" t="s">
+        <v>140</v>
+      </c>
+      <c r="G202" t="s">
+        <v>141</v>
+      </c>
+      <c r="H202" t="s">
+        <v>143</v>
+      </c>
+      <c r="I202" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9">
+      <c r="A203">
+        <f>1950-3800</f>
+        <v>-1850</v>
+      </c>
+      <c r="B203">
+        <f>(-41.60318611+-41.60318611)/2</f>
+        <v>-41.603186110000003</v>
+      </c>
+      <c r="C203">
+        <v>-38.369071699999999</v>
+      </c>
+      <c r="D203" t="s">
+        <v>139</v>
+      </c>
+      <c r="F203" t="s">
+        <v>140</v>
+      </c>
+      <c r="G203" t="s">
+        <v>141</v>
+      </c>
+      <c r="H203" t="s">
+        <v>144</v>
+      </c>
+      <c r="I203" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9">
+      <c r="A204">
+        <f>1950-3300</f>
+        <v>-1350</v>
+      </c>
+      <c r="B204">
+        <v>-39.816351660000002</v>
+      </c>
+      <c r="C204">
+        <v>-39.104548110000003</v>
+      </c>
+      <c r="D204" t="s">
+        <v>139</v>
+      </c>
+      <c r="F204" t="s">
+        <v>140</v>
+      </c>
+      <c r="G204" t="s">
+        <v>141</v>
+      </c>
+      <c r="H204" t="s">
+        <v>142</v>
+      </c>
+      <c r="I204" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="205" spans="1:9">
+      <c r="A205">
+        <f>1950-2200</f>
+        <v>-250</v>
+      </c>
+      <c r="B205">
+        <v>-41.743762969999999</v>
+      </c>
+      <c r="C205">
+        <v>-39.48480979</v>
+      </c>
+      <c r="D205" t="s">
+        <v>139</v>
+      </c>
+      <c r="F205" t="s">
+        <v>140</v>
+      </c>
+      <c r="G205" t="s">
+        <v>141</v>
+      </c>
+      <c r="H205" t="s">
+        <v>145</v>
+      </c>
+      <c r="I205" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9">
+      <c r="A206">
+        <f>1950-1800</f>
+        <v>150</v>
+      </c>
+      <c r="B206">
+        <v>-39.667778920000003</v>
+      </c>
+      <c r="C206">
+        <v>-38.369071699999999</v>
+      </c>
+      <c r="D206" t="s">
+        <v>139</v>
+      </c>
+      <c r="F206" t="s">
+        <v>140</v>
+      </c>
+      <c r="G206" t="s">
+        <v>141</v>
+      </c>
+      <c r="H206" t="s">
+        <v>143</v>
+      </c>
+      <c r="I206" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9">
+      <c r="A207">
+        <f>1950-1200</f>
+        <v>750</v>
+      </c>
+      <c r="B207">
+        <v>-40.82870535</v>
+      </c>
+      <c r="C207">
+        <v>-39.104548110000003</v>
+      </c>
+      <c r="D207" t="s">
+        <v>139</v>
+      </c>
+      <c r="F207" t="s">
+        <v>140</v>
+      </c>
+      <c r="G207" t="s">
+        <v>141</v>
+      </c>
+      <c r="H207" t="s">
+        <v>146</v>
+      </c>
+      <c r="I207" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="208" spans="1:9">
+      <c r="A208">
+        <f>1950-900</f>
+        <v>1050</v>
+      </c>
+      <c r="B208">
+        <v>-41.743762969999999</v>
+      </c>
+      <c r="C208">
+        <v>-38.369071699999999</v>
+      </c>
+      <c r="D208" t="s">
+        <v>139</v>
+      </c>
+      <c r="F208" t="s">
+        <v>140</v>
+      </c>
+      <c r="G208" t="s">
+        <v>141</v>
+      </c>
+      <c r="H208" t="s">
+        <v>147</v>
+      </c>
+      <c r="I208" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="209" spans="1:9">
+      <c r="A209">
+        <f>1950-500</f>
+        <v>1450</v>
+      </c>
+      <c r="B209">
+        <v>-41.743762969999999</v>
+      </c>
+      <c r="C209">
+        <v>-41.243539550000001</v>
+      </c>
+      <c r="D209" t="s">
+        <v>139</v>
+      </c>
+      <c r="F209" t="s">
+        <v>140</v>
+      </c>
+      <c r="G209" t="s">
+        <v>141</v>
+      </c>
+      <c r="H209" t="s">
+        <v>148</v>
+      </c>
+      <c r="I209" t="s">
+        <v>140</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>